<commit_message>
Correct data to be review
</commit_message>
<xml_diff>
--- a/data/resource/KHMT_lite.xlsx
+++ b/data/resource/KHMT_lite.xlsx
@@ -519,10 +519,15 @@
   <dimension ref="A1:G248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="J11" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="28.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>